<commit_message>
corrected request limit per host
</commit_message>
<xml_diff>
--- a/cars_data/cars.xlsx
+++ b/cars_data/cars.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>Гос номер</t>
   </si>
@@ -36,12 +36,6 @@
   </si>
   <si>
     <t>VIN</t>
-  </si>
-  <si>
-    <t>Гудвей "Москва"</t>
-  </si>
-  <si>
-    <t>Z94K241BBLR171290</t>
   </si>
   <si>
     <t>К296НА797</t>
@@ -525,7 +519,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -552,80 +546,128 @@
     </row>
     <row r="2" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>